<commit_message>
Update Extest User anme as Meraj
</commit_message>
<xml_diff>
--- a/src/test/java/com/Amazon/SearchData.xlsx
+++ b/src/test/java/com/Amazon/SearchData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Data</t>
   </si>
@@ -364,7 +364,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="46.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.5859375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.31640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>